<commit_message>
Fixed 8 out of 19 broken existing tests
</commit_message>
<xml_diff>
--- a/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template5.xlsx
+++ b/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\job_related\wegen_en_verkeer\new_python_otl_wizard\testData\simpel_vergelijkings_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\OTLMOW-GUI\demo_projects\simpel_vergelijkings_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E739F06-153D-4BB6-8E4D-F583A08DEBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0301645A-F7D4-4508-8DE4-41913CE1A54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ins#Verkeersbordopstelling" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,25 @@
     <sheet name="ond#LigtOp" sheetId="8" r:id="rId7"/>
     <sheet name="Keuzelijsten" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="242">
   <si>
     <t>typeURI</t>
   </si>
@@ -1117,11 +1130,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="19" width="20" customWidth="1"/>
   </cols>
@@ -1351,7 +1364,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="19" width="20" customWidth="1"/>
   </cols>
@@ -1569,7 +1582,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="13" width="20" customWidth="1"/>
   </cols>
@@ -1733,7 +1746,7 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="20" width="20" customWidth="1"/>
   </cols>
@@ -1962,17 +1975,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8E9B60-EC96-400E-94AB-803E6E938533}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="20.6328125" customWidth="1"/>
-    <col min="4" max="4" width="84.90625" customWidth="1"/>
-    <col min="5" max="6" width="20.6328125" customWidth="1"/>
-    <col min="7" max="7" width="24.08984375" customWidth="1"/>
-    <col min="8" max="19" width="20.6328125" customWidth="1"/>
+    <col min="1" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="84.85546875" customWidth="1"/>
+    <col min="5" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="19" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2012,31 +2025,31 @@
         <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
         <v>195</v>
       </c>
-      <c r="D2" t="s">
-        <v>65</v>
+      <c r="D2" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="F2" t="s">
         <v>197</v>
       </c>
-      <c r="G2" t="s">
-        <v>31</v>
+      <c r="G2" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>198</v>
       </c>
       <c r="I2" t="s">
         <v>199</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2044,31 +2057,31 @@
         <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>210</v>
+      <c r="D3" t="s">
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>196</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
         <v>197</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>209</v>
+      <c r="G3" t="s">
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>198</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
         <v>199</v>
       </c>
-      <c r="J3" t="b">
-        <v>1</v>
+      <c r="J3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2078,7 +2091,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" location="Bewegingssensor" xr:uid="{E2D0B29F-C478-42BB-9735-EEF8EEDE727A}"/>
+    <hyperlink ref="D2" r:id="rId1" location="Bewegingssensor" xr:uid="{E2D0B29F-C478-42BB-9735-EEF8EEDE727A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2089,12 +2102,12 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="26" width="20.6328125" customWidth="1"/>
+    <col min="1" max="26" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2175,13 +2188,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C37910F-4799-4014-9A7A-01BBA77DFC21}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="26" width="20.6328125" customWidth="1"/>
+    <col min="1" max="26" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2244,13 +2257,13 @@
       <c r="I2" t="s">
         <v>203</v>
       </c>
-      <c r="J2" t="b">
-        <v>0</v>
+      <c r="J2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="J2" xr:uid="{BC860AA8-DE2A-4F3C-BD78-6950880A9C34}">
+    <dataValidation type="list" allowBlank="1" sqref="J2" xr:uid="{CAEE14A6-078E-43CB-8A96-51B9D51C55B5}">
       <formula1>"TRUE,FALSE,-"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2269,7 +2282,7 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="700" width="20" customWidth="1"/>
   </cols>

</xml_diff>